<commit_message>
artcle 2 none finished
</commit_message>
<xml_diff>
--- a/参考文献.xlsx
+++ b/参考文献.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="4920" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_Ref507523414" localSheetId="0">Sheet1!$C$32</definedName>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="86">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -334,136 +335,125 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>光照不均匀图像的一种环带最优阈值分割方法</t>
+  </si>
+  <si>
+    <t>An Automated Fish Counting Algorithm in Aquaculture Based on Image Processing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Digitization of Free-Swimming Fish Based on Binocular Stereo Vision</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>徐立鸿,蔚瑞华,乐九一,曹家恒. 一种水产养殖的自动投饵和水质监测控制系统及方法[P]. 上海：CN107094683A,2017-08-29.</t>
+  </si>
+  <si>
+    <t>徐立鸿,蔚瑞华,曹家恒，张佳林. 一种基于计算机视觉的残留鱼饵计数方法[P]. 上海：CN109389613A，2017-08-29.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cao J, Xu L. Research on Counting Algorithm of Residual Feeds in Aquaculture Based on Machine Vision[C]//2018 IEEE 3rd International Conference on Image, Vision and Computing (ICIVC). IEEE, 2018: 498-503.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Eriksen M S, Faerevik G, Kittilsen S, et al. Stressed mothers–troubled offspring: a study of behavioural maternal effects in farmed Salmo salar[J]. Journal of fish biology, 2011, 79(3): 575-586.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高明学, 徐立鸿, 李大威,等. 光照不均匀图像的一种环带最优阈值分割方法[J]. 机电一体化, 2010, 16(2):26-30.</t>
+  </si>
+  <si>
+    <t>Ye Z, Zhao J, Han Z, et al. Behavioral characteristics and statistics-based imaging techniques in the assessment and optimization of tilapia feeding in a recirculating aquaculture system[J]. Transactions of the ASABE, 2016, 59(1): 345-355.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Docs.python.org. (2019). pickle — Python object serialization — Python 3.8.0 documentation. [online] Available at: https://docs.python.org/3/library/pickle.html [Accessed 23 Nov. 2019].</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>视频名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>异常</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>摄食</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>未摄食</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>开始时间1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>结束时间2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>结束时间1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>开始时间2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据类别</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G0715001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>##</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>##</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>##</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>##</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <r>
-      <t>高明学</t>
+      <t>"Lenna", </t>
     </r>
     <r>
       <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
-      <t xml:space="preserve">, </t>
+      <t>En.wikipedia.org</t>
     </r>
     <r>
       <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
-      <t>徐立鸿</t>
+      <t>, 2020. [Online]. Available: https://en.wikipedia.org/wiki/Lenna. [Accessed: 02- Jan- 2020].</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>李大威</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>等</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>光照不均匀图像的一种环带最优阈值分割方法</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">[J]. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>机电一体化</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, 2010, 16(2):26-30.</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>光照不均匀图像的一种环带最优阈值分割方法</t>
-  </si>
-  <si>
-    <t>An Automated Fish Counting Algorithm in Aquaculture Based on Image Processing</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Digitization of Free-Swimming Fish Based on Binocular Stereo Vision</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>徐立鸿,蔚瑞华,乐九一,曹家恒. 一种水产养殖的自动投饵和水质监测控制系统及方法[P]. 上海：CN107094683A,2017-08-29.</t>
-  </si>
-  <si>
-    <t>徐立鸿,蔚瑞华,曹家恒，张佳林. 一种基于计算机视觉的残留鱼饵计数方法[P]. 上海：CN109389613A，2017-08-29.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cao J, Xu L. Research on Counting Algorithm of Residual Feeds in Aquaculture Based on Machine Vision[C]//2018 IEEE 3rd International Conference on Image, Vision and Computing (ICIVC). IEEE, 2018: 498-503.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shanon C. A mathematical theory of communication[J]. Bell System Technical Journal, 1948, 27: 379-623.</t>
   </si>
 </sst>
 </file>
@@ -531,17 +521,17 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10.5"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="10.5"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -552,7 +542,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -560,11 +550,146 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -574,6 +699,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -857,7 +1009,7 @@
   <dimension ref="A1:D170"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -1124,7 +1276,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -1205,7 +1357,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>59</v>
@@ -1216,29 +1368,29 @@
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A34" s="5">
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>34</v>
       </c>
-      <c r="C35" s="6" t="s">
-        <v>66</v>
+      <c r="C35" s="3" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.15">
@@ -1246,7 +1398,7 @@
         <v>35</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.15">
@@ -1254,32 +1406,47 @@
         <v>36</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C38" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C39" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C40" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C41" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="5">
         <v>41</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.15">
@@ -1927,4 +2094,100 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:G5"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B2" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B3" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B4" s="7"/>
+      <c r="C4" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="12">
+        <v>25</v>
+      </c>
+      <c r="E4" s="12">
+        <v>55</v>
+      </c>
+      <c r="F4" s="12">
+        <v>100</v>
+      </c>
+      <c r="G4" s="13">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="8"/>
+      <c r="C5" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="14">
+        <v>0</v>
+      </c>
+      <c r="E5" s="14">
+        <v>25</v>
+      </c>
+      <c r="F5" s="14">
+        <v>55</v>
+      </c>
+      <c r="G5" s="15">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:B5"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>